<commit_message>
successful test execution commit
</commit_message>
<xml_diff>
--- a/testdata/testdata.xlsx
+++ b/testdata/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lallu/Downloads/Repositories/Work/seleniumtestngframework/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B95715C6-0AE2-8543-A874-4A2A69098B31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D00A539B-3FBF-7C49-86AA-C2D8E78AAC93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="740" windowWidth="24960" windowHeight="17260" xr2:uid="{A5EA2BDE-0F4B-704F-ADDD-D46A291F8767}"/>
+    <workbookView xWindow="4680" yWindow="740" windowWidth="24960" windowHeight="17260" xr2:uid="{A5EA2BDE-0F4B-704F-ADDD-D46A291F8767}"/>
   </bookViews>
   <sheets>
     <sheet name="FormData" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>FirstName</t>
   </si>
@@ -102,6 +102,12 @@
   </si>
   <si>
     <t>Navigation Commands</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
   </si>
 </sst>
 </file>
@@ -144,9 +150,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -484,7 +491,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -535,8 +542,8 @@
       <c r="C2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D2">
-        <v>5</v>
+      <c r="D2" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>11</v>
@@ -561,8 +568,8 @@
       <c r="C3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D3">
-        <v>7</v>
+      <c r="D3" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>18</v>

</xml_diff>